<commit_message>
Update List of Table Number_07122024.xlsx
</commit_message>
<xml_diff>
--- a/List of Table Number_07122024.xlsx
+++ b/List of Table Number_07122024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\US\Documents\GitHub\gitddinner2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CF1B44-E9CF-41EC-B802-89597F80645A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E96A167-D49C-4C4C-BC27-0BFDE05D7498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{39DB9A1F-5381-4974-925D-A22F547FBD30}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{39DB9A1F-5381-4974-925D-A22F547FBD30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="990">
   <si>
     <t>GITD</t>
   </si>
@@ -1999,9 +1999,6 @@
     <t>S53714</t>
   </si>
   <si>
-    <t>M11692</t>
-  </si>
-  <si>
     <t>TM39867</t>
   </si>
   <si>
@@ -2653,9 +2650,6 @@
     <t>TM30136</t>
   </si>
   <si>
-    <t>C0680</t>
-  </si>
-  <si>
     <t>S53151</t>
   </si>
   <si>
@@ -3002,13 +2996,22 @@
   </si>
   <si>
     <t>DIV</t>
+  </si>
+  <si>
+    <t>GN0263</t>
+  </si>
+  <si>
+    <t>TM40345</t>
+  </si>
+  <si>
+    <t>VC0680</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3100,6 +3103,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -3183,7 +3194,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3293,6 +3304,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3615,8 +3629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F279ECC-7305-4F31-A260-4783CCF1EFAD}">
   <dimension ref="A1:E460"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A411" workbookViewId="0">
+      <selection activeCell="C411" sqref="C411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3633,7 +3647,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>15</v>
@@ -3659,7 +3673,7 @@
         <v>538</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3673,10 +3687,10 @@
         <v>17</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3693,7 +3707,7 @@
         <v>539</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3710,7 +3724,7 @@
         <v>540</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3846,7 +3860,7 @@
         <v>548</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3880,7 +3894,7 @@
         <v>550</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3931,7 +3945,7 @@
         <v>553</v>
       </c>
       <c r="E18" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3948,7 +3962,7 @@
         <v>554</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3965,7 +3979,7 @@
         <v>555</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3982,7 +3996,7 @@
         <v>556</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3999,7 +4013,7 @@
         <v>557</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -4033,7 +4047,7 @@
         <v>559</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -4050,7 +4064,7 @@
         <v>560</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -4084,7 +4098,7 @@
         <v>562</v>
       </c>
       <c r="E27" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -4118,7 +4132,7 @@
         <v>564</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -4152,7 +4166,7 @@
         <v>566</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -4203,7 +4217,7 @@
         <v>569</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4237,7 +4251,7 @@
         <v>571</v>
       </c>
       <c r="E36" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -4254,7 +4268,7 @@
         <v>572</v>
       </c>
       <c r="E37" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -4356,7 +4370,7 @@
         <v>578</v>
       </c>
       <c r="E43" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -4424,7 +4438,7 @@
         <v>582</v>
       </c>
       <c r="E47" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4441,7 +4455,7 @@
         <v>583</v>
       </c>
       <c r="E48" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -4458,7 +4472,7 @@
         <v>584</v>
       </c>
       <c r="E49" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4475,7 +4489,7 @@
         <v>585</v>
       </c>
       <c r="E50" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -4492,7 +4506,7 @@
         <v>586</v>
       </c>
       <c r="E51" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -4526,7 +4540,7 @@
         <v>588</v>
       </c>
       <c r="E53" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -4543,7 +4557,7 @@
         <v>589</v>
       </c>
       <c r="E54" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -4645,7 +4659,7 @@
         <v>595</v>
       </c>
       <c r="E60" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -4662,7 +4676,7 @@
         <v>596</v>
       </c>
       <c r="E61" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -4679,7 +4693,7 @@
         <v>597</v>
       </c>
       <c r="E62" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -4730,7 +4744,7 @@
         <v>600</v>
       </c>
       <c r="E65" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -4764,7 +4778,7 @@
         <v>602</v>
       </c>
       <c r="E67" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -4781,7 +4795,7 @@
         <v>603</v>
       </c>
       <c r="E68" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -4832,7 +4846,7 @@
         <v>606</v>
       </c>
       <c r="E71" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -4849,7 +4863,7 @@
         <v>607</v>
       </c>
       <c r="E72" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -4866,7 +4880,7 @@
         <v>608</v>
       </c>
       <c r="E73" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4883,7 +4897,7 @@
         <v>609</v>
       </c>
       <c r="E74" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -4917,7 +4931,7 @@
         <v>611</v>
       </c>
       <c r="E76" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -4985,7 +4999,7 @@
         <v>615</v>
       </c>
       <c r="E80" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -5002,7 +5016,7 @@
         <v>616</v>
       </c>
       <c r="E81" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -5019,7 +5033,7 @@
         <v>617</v>
       </c>
       <c r="E82" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -5053,7 +5067,7 @@
         <v>619</v>
       </c>
       <c r="E84" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -5070,7 +5084,7 @@
         <v>620</v>
       </c>
       <c r="E85" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -5087,7 +5101,7 @@
         <v>621</v>
       </c>
       <c r="E86" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -5121,7 +5135,7 @@
         <v>623</v>
       </c>
       <c r="E88" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -5155,7 +5169,7 @@
         <v>625</v>
       </c>
       <c r="E90" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -5172,7 +5186,7 @@
         <v>626</v>
       </c>
       <c r="E91" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -5189,7 +5203,7 @@
         <v>627</v>
       </c>
       <c r="E92" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -5223,7 +5237,7 @@
         <v>629</v>
       </c>
       <c r="E94" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -5240,7 +5254,7 @@
         <v>630</v>
       </c>
       <c r="E95" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -5274,7 +5288,7 @@
         <v>632</v>
       </c>
       <c r="E97" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -5291,7 +5305,7 @@
         <v>633</v>
       </c>
       <c r="E98" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -5308,7 +5322,7 @@
         <v>634</v>
       </c>
       <c r="E99" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -5325,7 +5339,7 @@
         <v>635</v>
       </c>
       <c r="E100" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -5342,7 +5356,7 @@
         <v>636</v>
       </c>
       <c r="E101" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -5359,7 +5373,7 @@
         <v>637</v>
       </c>
       <c r="E102" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -5427,7 +5441,7 @@
         <v>641</v>
       </c>
       <c r="E106" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -5512,7 +5526,7 @@
         <v>646</v>
       </c>
       <c r="E111" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -5529,7 +5543,7 @@
         <v>647</v>
       </c>
       <c r="E112" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -5563,7 +5577,7 @@
         <v>649</v>
       </c>
       <c r="E114" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -5580,7 +5594,7 @@
         <v>650</v>
       </c>
       <c r="E115" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -5597,7 +5611,7 @@
         <v>651</v>
       </c>
       <c r="E116" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -5614,7 +5628,7 @@
         <v>652</v>
       </c>
       <c r="E117" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -5631,7 +5645,7 @@
         <v>653</v>
       </c>
       <c r="E118" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -5644,11 +5658,11 @@
       <c r="C119" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D119" s="31" t="s">
-        <v>654</v>
+      <c r="D119" s="42" t="s">
+        <v>988</v>
       </c>
       <c r="E119" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -5662,10 +5676,10 @@
         <v>134</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="E120" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -5679,10 +5693,10 @@
         <v>135</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E121" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -5696,10 +5710,10 @@
         <v>136</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="E122" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -5713,10 +5727,10 @@
         <v>137</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="E123" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -5730,7 +5744,7 @@
         <v>138</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E124" s="40">
         <v>8</v>
@@ -5747,10 +5761,10 @@
         <v>139</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="E125" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -5764,10 +5778,10 @@
         <v>140</v>
       </c>
       <c r="D126" s="31" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E126" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -5781,10 +5795,10 @@
         <v>141</v>
       </c>
       <c r="D127" s="31" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E127" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -5798,10 +5812,10 @@
         <v>142</v>
       </c>
       <c r="D128" s="31" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E128" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -5815,7 +5829,7 @@
         <v>143</v>
       </c>
       <c r="D129" s="31" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E129" s="40">
         <v>14</v>
@@ -5832,7 +5846,7 @@
         <v>144</v>
       </c>
       <c r="D130" s="31" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E130" s="40">
         <v>12</v>
@@ -5849,7 +5863,7 @@
         <v>145</v>
       </c>
       <c r="D131" s="31" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E131" s="40">
         <v>14</v>
@@ -5866,7 +5880,7 @@
         <v>146</v>
       </c>
       <c r="D132" s="31" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E132" s="40">
         <v>14</v>
@@ -5883,7 +5897,7 @@
         <v>147</v>
       </c>
       <c r="D133" s="31" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E133" s="40">
         <v>14</v>
@@ -5900,10 +5914,10 @@
         <v>148</v>
       </c>
       <c r="D134" s="31" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E134" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -5917,10 +5931,10 @@
         <v>149</v>
       </c>
       <c r="D135" s="31" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E135" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -5934,7 +5948,7 @@
         <v>150</v>
       </c>
       <c r="D136" s="31" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E136" s="40">
         <v>12</v>
@@ -5951,10 +5965,10 @@
         <v>151</v>
       </c>
       <c r="D137" s="31" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E137" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -5968,7 +5982,7 @@
         <v>152</v>
       </c>
       <c r="D138" s="31" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E138" s="40">
         <v>3</v>
@@ -5985,7 +5999,7 @@
         <v>153</v>
       </c>
       <c r="D139" s="31" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E139" s="40">
         <v>1</v>
@@ -6002,10 +6016,10 @@
         <v>154</v>
       </c>
       <c r="D140" s="31" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E140" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -6019,7 +6033,7 @@
         <v>155</v>
       </c>
       <c r="D141" s="31" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E141" s="40">
         <v>3</v>
@@ -6036,7 +6050,7 @@
         <v>156</v>
       </c>
       <c r="D142" s="31" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E142" s="40">
         <v>3</v>
@@ -6053,10 +6067,10 @@
         <v>157</v>
       </c>
       <c r="D143" s="31" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E143" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -6070,7 +6084,7 @@
         <v>158</v>
       </c>
       <c r="D144" s="31" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E144" s="40">
         <v>3</v>
@@ -6087,7 +6101,7 @@
         <v>159</v>
       </c>
       <c r="D145" s="31" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E145" s="40">
         <v>3</v>
@@ -6104,10 +6118,10 @@
         <v>160</v>
       </c>
       <c r="D146" s="31" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E146" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -6121,7 +6135,7 @@
         <v>161</v>
       </c>
       <c r="D147" s="31" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E147" s="40">
         <v>3</v>
@@ -6138,10 +6152,10 @@
         <v>162</v>
       </c>
       <c r="D148" s="31" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E148" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -6155,7 +6169,7 @@
         <v>163</v>
       </c>
       <c r="D149" s="31" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E149" s="40">
         <v>6</v>
@@ -6172,10 +6186,10 @@
         <v>164</v>
       </c>
       <c r="D150" s="31" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E150" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -6189,10 +6203,10 @@
         <v>165</v>
       </c>
       <c r="D151" s="31" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E151" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -6206,10 +6220,10 @@
         <v>166</v>
       </c>
       <c r="D152" s="31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E152" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -6223,10 +6237,10 @@
         <v>167</v>
       </c>
       <c r="D153" s="31" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E153" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -6240,10 +6254,10 @@
         <v>168</v>
       </c>
       <c r="D154" s="31" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E154" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -6257,10 +6271,10 @@
         <v>169</v>
       </c>
       <c r="D155" s="31" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E155" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -6274,10 +6288,10 @@
         <v>170</v>
       </c>
       <c r="D156" s="31" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E156" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -6291,10 +6305,10 @@
         <v>171</v>
       </c>
       <c r="D157" s="31" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E157" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -6308,10 +6322,10 @@
         <v>172</v>
       </c>
       <c r="D158" s="31" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E158" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -6325,10 +6339,10 @@
         <v>173</v>
       </c>
       <c r="D159" s="31" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E159" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -6342,10 +6356,10 @@
         <v>174</v>
       </c>
       <c r="D160" s="31" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E160" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -6359,10 +6373,10 @@
         <v>175</v>
       </c>
       <c r="D161" s="31" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E161" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -6376,10 +6390,10 @@
         <v>176</v>
       </c>
       <c r="D162" s="31" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E162" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -6393,10 +6407,10 @@
         <v>177</v>
       </c>
       <c r="D163" s="31" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E163" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -6410,10 +6424,10 @@
         <v>178</v>
       </c>
       <c r="D164" s="31" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E164" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -6427,10 +6441,10 @@
         <v>179</v>
       </c>
       <c r="D165" s="31" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E165" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -6444,10 +6458,10 @@
         <v>180</v>
       </c>
       <c r="D166" s="31" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E166" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -6461,10 +6475,10 @@
         <v>181</v>
       </c>
       <c r="D167" s="31" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E167" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -6478,10 +6492,10 @@
         <v>182</v>
       </c>
       <c r="D168" s="31" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E168" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -6495,10 +6509,10 @@
         <v>183</v>
       </c>
       <c r="D169" s="31" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E169" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -6512,10 +6526,10 @@
         <v>184</v>
       </c>
       <c r="D170" s="31" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E170" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -6529,10 +6543,10 @@
         <v>185</v>
       </c>
       <c r="D171" s="31" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E171" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -6546,7 +6560,7 @@
         <v>186</v>
       </c>
       <c r="D172" s="31" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E172" s="40">
         <v>3</v>
@@ -6563,7 +6577,7 @@
         <v>187</v>
       </c>
       <c r="D173" s="31" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E173" s="40">
         <v>3</v>
@@ -6580,7 +6594,7 @@
         <v>188</v>
       </c>
       <c r="D174" s="31" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E174" s="40">
         <v>3</v>
@@ -6597,10 +6611,10 @@
         <v>189</v>
       </c>
       <c r="D175" s="31" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E175" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -6614,7 +6628,7 @@
         <v>190</v>
       </c>
       <c r="D176" s="31" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E176" s="40">
         <v>7</v>
@@ -6631,7 +6645,7 @@
         <v>191</v>
       </c>
       <c r="D177" s="31" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E177" s="40">
         <v>6</v>
@@ -6648,10 +6662,10 @@
         <v>192</v>
       </c>
       <c r="D178" s="31" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E178" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -6665,10 +6679,10 @@
         <v>193</v>
       </c>
       <c r="D179" s="31" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E179" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -6682,10 +6696,10 @@
         <v>194</v>
       </c>
       <c r="D180" s="31" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E180" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -6699,10 +6713,10 @@
         <v>195</v>
       </c>
       <c r="D181" s="31" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E181" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -6716,10 +6730,10 @@
         <v>196</v>
       </c>
       <c r="D182" s="31" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E182" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -6733,10 +6747,10 @@
         <v>197</v>
       </c>
       <c r="D183" s="31" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E183" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -6750,10 +6764,10 @@
         <v>198</v>
       </c>
       <c r="D184" s="31" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E184" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -6767,10 +6781,10 @@
         <v>199</v>
       </c>
       <c r="D185" s="31" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="E185" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -6784,10 +6798,10 @@
         <v>200</v>
       </c>
       <c r="D186" s="31" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="E186" s="41" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -6801,7 +6815,7 @@
         <v>201</v>
       </c>
       <c r="D187" s="31" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="E187" s="40">
         <v>6</v>
@@ -6818,10 +6832,10 @@
         <v>202</v>
       </c>
       <c r="D188" s="31" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E188" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -6835,10 +6849,10 @@
         <v>203</v>
       </c>
       <c r="D189" s="31" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E189" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -6852,10 +6866,10 @@
         <v>204</v>
       </c>
       <c r="D190" s="31" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E190" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -6869,10 +6883,10 @@
         <v>205</v>
       </c>
       <c r="D191" s="31" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="E191" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -6886,10 +6900,10 @@
         <v>206</v>
       </c>
       <c r="D192" s="31" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="E192" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -6903,10 +6917,10 @@
         <v>207</v>
       </c>
       <c r="D193" s="31" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E193" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -6920,10 +6934,10 @@
         <v>208</v>
       </c>
       <c r="D194" s="31" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E194" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -6937,7 +6951,7 @@
         <v>209</v>
       </c>
       <c r="D195" s="31" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E195" s="40">
         <v>1</v>
@@ -6954,7 +6968,7 @@
         <v>210</v>
       </c>
       <c r="D196" s="31" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E196" s="40">
         <v>1</v>
@@ -6971,10 +6985,10 @@
         <v>211</v>
       </c>
       <c r="D197" s="31" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E197" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -6988,10 +7002,10 @@
         <v>212</v>
       </c>
       <c r="D198" s="31" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E198" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -7005,10 +7019,10 @@
         <v>213</v>
       </c>
       <c r="D199" s="31" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E199" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -7022,10 +7036,10 @@
         <v>214</v>
       </c>
       <c r="D200" s="31" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E200" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -7039,10 +7053,10 @@
         <v>215</v>
       </c>
       <c r="D201" s="31" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="E201" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -7056,10 +7070,10 @@
         <v>216</v>
       </c>
       <c r="D202" s="31" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E202" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -7073,10 +7087,10 @@
         <v>217</v>
       </c>
       <c r="D203" s="31" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E203" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -7090,10 +7104,10 @@
         <v>218</v>
       </c>
       <c r="D204" s="31" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E204" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -7107,10 +7121,10 @@
         <v>219</v>
       </c>
       <c r="D205" s="31" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="E205" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -7124,10 +7138,10 @@
         <v>220</v>
       </c>
       <c r="D206" s="31" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E206" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -7141,10 +7155,10 @@
         <v>221</v>
       </c>
       <c r="D207" s="31" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E207" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -7158,10 +7172,10 @@
         <v>222</v>
       </c>
       <c r="D208" s="31" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="E208" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -7175,10 +7189,10 @@
         <v>223</v>
       </c>
       <c r="D209" s="31" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E209" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -7192,10 +7206,10 @@
         <v>224</v>
       </c>
       <c r="D210" s="31" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="E210" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -7209,10 +7223,10 @@
         <v>225</v>
       </c>
       <c r="D211" s="31" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E211" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -7226,10 +7240,10 @@
         <v>226</v>
       </c>
       <c r="D212" s="31" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="E212" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -7243,10 +7257,10 @@
         <v>227</v>
       </c>
       <c r="D213" s="31" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="E213" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -7260,10 +7274,10 @@
         <v>228</v>
       </c>
       <c r="D214" s="31" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E214" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -7277,10 +7291,10 @@
         <v>229</v>
       </c>
       <c r="D215" s="31" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="E215" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -7294,10 +7308,10 @@
         <v>230</v>
       </c>
       <c r="D216" s="31" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="E216" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -7311,7 +7325,7 @@
         <v>231</v>
       </c>
       <c r="D217" s="31" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E217" s="40">
         <v>1</v>
@@ -7328,10 +7342,10 @@
         <v>232</v>
       </c>
       <c r="D218" s="31" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="E218" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -7345,10 +7359,10 @@
         <v>233</v>
       </c>
       <c r="D219" s="31" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E219" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -7362,10 +7376,10 @@
         <v>234</v>
       </c>
       <c r="D220" s="31" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="E220" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -7379,10 +7393,10 @@
         <v>235</v>
       </c>
       <c r="D221" s="31" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="E221" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -7396,10 +7410,10 @@
         <v>236</v>
       </c>
       <c r="D222" s="31" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="E222" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -7413,10 +7427,10 @@
         <v>237</v>
       </c>
       <c r="D223" s="31" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="E223" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -7430,7 +7444,7 @@
         <v>238</v>
       </c>
       <c r="D224" s="31" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E224" s="40">
         <v>4</v>
@@ -7447,7 +7461,7 @@
         <v>239</v>
       </c>
       <c r="D225" s="31" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="E225" s="40">
         <v>4</v>
@@ -7464,10 +7478,10 @@
         <v>240</v>
       </c>
       <c r="D226" s="31" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="E226" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -7481,10 +7495,10 @@
         <v>241</v>
       </c>
       <c r="D227" s="31" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="E227" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -7498,10 +7512,10 @@
         <v>242</v>
       </c>
       <c r="D228" s="31" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E228" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -7515,10 +7529,10 @@
         <v>243</v>
       </c>
       <c r="D229" s="31" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="E229" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -7532,10 +7546,10 @@
         <v>244</v>
       </c>
       <c r="D230" s="31" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E230" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -7549,7 +7563,7 @@
         <v>245</v>
       </c>
       <c r="D231" s="31" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E231" s="40">
         <v>4</v>
@@ -7566,7 +7580,7 @@
         <v>246</v>
       </c>
       <c r="D232" s="31" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="E232" s="40">
         <v>4</v>
@@ -7583,10 +7597,10 @@
         <v>247</v>
       </c>
       <c r="D233" s="31" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E233" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -7600,10 +7614,10 @@
         <v>248</v>
       </c>
       <c r="D234" s="31" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="E234" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -7617,10 +7631,10 @@
         <v>249</v>
       </c>
       <c r="D235" s="31" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E235" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -7634,10 +7648,10 @@
         <v>250</v>
       </c>
       <c r="D236" s="31" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E236" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -7651,10 +7665,10 @@
         <v>251</v>
       </c>
       <c r="D237" s="31" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E237" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -7668,7 +7682,7 @@
         <v>252</v>
       </c>
       <c r="D238" s="31" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E238" s="40">
         <v>1</v>
@@ -7685,10 +7699,10 @@
         <v>253</v>
       </c>
       <c r="D239" s="31" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E239" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -7702,10 +7716,10 @@
         <v>254</v>
       </c>
       <c r="D240" s="31" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E240" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -7719,10 +7733,10 @@
         <v>255</v>
       </c>
       <c r="D241" s="31" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E241" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -7736,7 +7750,7 @@
         <v>256</v>
       </c>
       <c r="D242" s="31" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E242" s="40">
         <v>18</v>
@@ -7753,7 +7767,7 @@
         <v>257</v>
       </c>
       <c r="D243" s="31" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="E243" s="40">
         <v>18</v>
@@ -7770,10 +7784,10 @@
         <v>258</v>
       </c>
       <c r="D244" s="31" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E244" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -7787,10 +7801,10 @@
         <v>259</v>
       </c>
       <c r="D245" s="31" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E245" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -7804,7 +7818,7 @@
         <v>260</v>
       </c>
       <c r="D246" s="31" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E246" s="40">
         <v>18</v>
@@ -7821,7 +7835,7 @@
         <v>261</v>
       </c>
       <c r="D247" s="31" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="E247" s="40">
         <v>18</v>
@@ -7838,7 +7852,7 @@
         <v>262</v>
       </c>
       <c r="D248" s="31" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E248" s="40">
         <v>18</v>
@@ -7855,10 +7869,10 @@
         <v>263</v>
       </c>
       <c r="D249" s="31" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E249" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -7872,10 +7886,10 @@
         <v>264</v>
       </c>
       <c r="D250" s="31" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E250" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -7889,10 +7903,10 @@
         <v>265</v>
       </c>
       <c r="D251" s="31" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E251" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -7906,10 +7920,10 @@
         <v>266</v>
       </c>
       <c r="D252" s="31" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="E252" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -7923,10 +7937,10 @@
         <v>267</v>
       </c>
       <c r="D253" s="31" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E253" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -7940,10 +7954,10 @@
         <v>268</v>
       </c>
       <c r="D254" s="31" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E254" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -7957,10 +7971,10 @@
         <v>269</v>
       </c>
       <c r="D255" s="31" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E255" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -7974,10 +7988,10 @@
         <v>270</v>
       </c>
       <c r="D256" s="31" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="E256" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -7991,10 +8005,10 @@
         <v>271</v>
       </c>
       <c r="D257" s="31" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="E257" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -8008,10 +8022,10 @@
         <v>272</v>
       </c>
       <c r="D258" s="31" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E258" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -8025,10 +8039,10 @@
         <v>273</v>
       </c>
       <c r="D259" s="31" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E259" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -8042,10 +8056,10 @@
         <v>274</v>
       </c>
       <c r="D260" s="31" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E260" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -8059,10 +8073,10 @@
         <v>275</v>
       </c>
       <c r="D261" s="31" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E261" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -8076,10 +8090,10 @@
         <v>276</v>
       </c>
       <c r="D262" s="31" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E262" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -8093,10 +8107,10 @@
         <v>277</v>
       </c>
       <c r="D263" s="31" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E263" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -8110,10 +8124,10 @@
         <v>278</v>
       </c>
       <c r="D264" s="31" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E264" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -8127,10 +8141,10 @@
         <v>279</v>
       </c>
       <c r="D265" s="31" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E265" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -8144,10 +8158,10 @@
         <v>280</v>
       </c>
       <c r="D266" s="31" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E266" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -8161,7 +8175,7 @@
         <v>281</v>
       </c>
       <c r="D267" s="31" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E267" s="40">
         <v>1</v>
@@ -8178,7 +8192,7 @@
         <v>282</v>
       </c>
       <c r="D268" s="31" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E268" s="40">
         <v>1</v>
@@ -8195,10 +8209,10 @@
         <v>283</v>
       </c>
       <c r="D269" s="31" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E269" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -8212,10 +8226,10 @@
         <v>284</v>
       </c>
       <c r="D270" s="31" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E270" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -8229,10 +8243,10 @@
         <v>285</v>
       </c>
       <c r="D271" s="31" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E271" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -8246,10 +8260,10 @@
         <v>286</v>
       </c>
       <c r="D272" s="31" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E272" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -8263,10 +8277,10 @@
         <v>287</v>
       </c>
       <c r="D273" s="31" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E273" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -8280,10 +8294,10 @@
         <v>288</v>
       </c>
       <c r="D274" s="31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E274" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -8297,10 +8311,10 @@
         <v>289</v>
       </c>
       <c r="D275" s="31" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E275" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -8314,7 +8328,7 @@
         <v>290</v>
       </c>
       <c r="D276" s="31" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E276" s="40">
         <v>15</v>
@@ -8331,7 +8345,7 @@
         <v>291</v>
       </c>
       <c r="D277" s="31" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E277" s="40">
         <v>15</v>
@@ -8348,10 +8362,10 @@
         <v>292</v>
       </c>
       <c r="D278" s="31" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E278" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -8365,10 +8379,10 @@
         <v>293</v>
       </c>
       <c r="D279" s="31" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E279" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
@@ -8382,7 +8396,7 @@
         <v>294</v>
       </c>
       <c r="D280" s="31" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E280" s="40">
         <v>11</v>
@@ -8399,7 +8413,7 @@
         <v>295</v>
       </c>
       <c r="D281" s="31" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E281" s="40">
         <v>11</v>
@@ -8416,7 +8430,7 @@
         <v>296</v>
       </c>
       <c r="D282" s="31" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E282" s="40">
         <v>11</v>
@@ -8433,7 +8447,7 @@
         <v>297</v>
       </c>
       <c r="D283" s="31" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E283" s="40">
         <v>11</v>
@@ -8450,7 +8464,7 @@
         <v>298</v>
       </c>
       <c r="D284" s="31" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E284" s="40">
         <v>17</v>
@@ -8467,7 +8481,7 @@
         <v>299</v>
       </c>
       <c r="D285" s="31" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E285" s="40">
         <v>17</v>
@@ -8484,7 +8498,7 @@
         <v>300</v>
       </c>
       <c r="D286" s="31" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E286" s="40">
         <v>17</v>
@@ -8501,7 +8515,7 @@
         <v>301</v>
       </c>
       <c r="D287" s="31" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E287" s="40">
         <v>17</v>
@@ -8518,7 +8532,7 @@
         <v>302</v>
       </c>
       <c r="D288" s="31" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E288" s="40">
         <v>11</v>
@@ -8535,10 +8549,10 @@
         <v>303</v>
       </c>
       <c r="D289" s="31" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E289" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -8552,7 +8566,7 @@
         <v>304</v>
       </c>
       <c r="D290" s="31" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E290" s="40">
         <v>16</v>
@@ -8569,7 +8583,7 @@
         <v>305</v>
       </c>
       <c r="D291" s="31" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E291" s="40">
         <v>11</v>
@@ -8586,7 +8600,7 @@
         <v>306</v>
       </c>
       <c r="D292" s="31" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="E292" s="40">
         <v>11</v>
@@ -8603,7 +8617,7 @@
         <v>307</v>
       </c>
       <c r="D293" s="31" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E293" s="40">
         <v>16</v>
@@ -8620,10 +8634,10 @@
         <v>308</v>
       </c>
       <c r="D294" s="31" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E294" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -8637,10 +8651,10 @@
         <v>309</v>
       </c>
       <c r="D295" s="31" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E295" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -8654,10 +8668,10 @@
         <v>310</v>
       </c>
       <c r="D296" s="31" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E296" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -8671,10 +8685,10 @@
         <v>311</v>
       </c>
       <c r="D297" s="31" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E297" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -8688,10 +8702,10 @@
         <v>312</v>
       </c>
       <c r="D298" s="31" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E298" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -8705,10 +8719,10 @@
         <v>313</v>
       </c>
       <c r="D299" s="31" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E299" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -8722,10 +8736,10 @@
         <v>314</v>
       </c>
       <c r="D300" s="31" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="E300" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -8739,10 +8753,10 @@
         <v>315</v>
       </c>
       <c r="D301" s="31" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E301" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -8756,10 +8770,10 @@
         <v>316</v>
       </c>
       <c r="D302" s="31" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="E302" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -8773,10 +8787,10 @@
         <v>317</v>
       </c>
       <c r="D303" s="31" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="E303" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
@@ -8790,10 +8804,10 @@
         <v>318</v>
       </c>
       <c r="D304" s="31" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E304" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -8807,10 +8821,10 @@
         <v>319</v>
       </c>
       <c r="D305" s="31" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="E305" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -8824,10 +8838,10 @@
         <v>320</v>
       </c>
       <c r="D306" s="31" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E306" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -8841,7 +8855,7 @@
         <v>321</v>
       </c>
       <c r="D307" s="31" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="E307" s="40">
         <v>12</v>
@@ -8858,7 +8872,7 @@
         <v>322</v>
       </c>
       <c r="D308" s="31" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E308" s="40">
         <v>9</v>
@@ -8875,10 +8889,10 @@
         <v>323</v>
       </c>
       <c r="D309" s="31" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E309" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -8892,10 +8906,10 @@
         <v>324</v>
       </c>
       <c r="D310" s="31" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="E310" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -8909,7 +8923,7 @@
         <v>325</v>
       </c>
       <c r="D311" s="31" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E311" s="40">
         <v>12</v>
@@ -8926,7 +8940,7 @@
         <v>326</v>
       </c>
       <c r="D312" s="31" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E312" s="40">
         <v>9</v>
@@ -8943,7 +8957,7 @@
         <v>327</v>
       </c>
       <c r="D313" s="31" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E313" s="40">
         <v>9</v>
@@ -8960,10 +8974,10 @@
         <v>328</v>
       </c>
       <c r="D314" s="31" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E314" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
@@ -8977,10 +8991,10 @@
         <v>329</v>
       </c>
       <c r="D315" s="31" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E315" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
@@ -8994,7 +9008,7 @@
         <v>330</v>
       </c>
       <c r="D316" s="31" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E316" s="40">
         <v>8</v>
@@ -9011,7 +9025,7 @@
         <v>331</v>
       </c>
       <c r="D317" s="31" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E317" s="40">
         <v>8</v>
@@ -9028,10 +9042,10 @@
         <v>332</v>
       </c>
       <c r="D318" s="31" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E318" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
@@ -9045,10 +9059,10 @@
         <v>333</v>
       </c>
       <c r="D319" s="31" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E319" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
@@ -9062,7 +9076,7 @@
         <v>334</v>
       </c>
       <c r="D320" s="31" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E320" s="40">
         <v>15</v>
@@ -9079,7 +9093,7 @@
         <v>335</v>
       </c>
       <c r="D321" s="31" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E321" s="40">
         <v>12</v>
@@ -9096,10 +9110,10 @@
         <v>336</v>
       </c>
       <c r="D322" s="31" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E322" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
@@ -9113,7 +9127,7 @@
         <v>337</v>
       </c>
       <c r="D323" s="31" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E323" s="40">
         <v>15</v>
@@ -9130,7 +9144,7 @@
         <v>338</v>
       </c>
       <c r="D324" s="31" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E324" s="40">
         <v>15</v>
@@ -9147,10 +9161,10 @@
         <v>339</v>
       </c>
       <c r="D325" s="31" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E325" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="326" spans="1:5" x14ac:dyDescent="0.25">
@@ -9164,10 +9178,10 @@
         <v>340</v>
       </c>
       <c r="D326" s="31" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E326" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
@@ -9181,7 +9195,7 @@
         <v>341</v>
       </c>
       <c r="D327" s="31" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="E327" s="40">
         <v>10</v>
@@ -9198,10 +9212,10 @@
         <v>342</v>
       </c>
       <c r="D328" s="31" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E328" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -9215,7 +9229,7 @@
         <v>343</v>
       </c>
       <c r="D329" s="31" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E329" s="40">
         <v>6</v>
@@ -9232,10 +9246,10 @@
         <v>344</v>
       </c>
       <c r="D330" s="31" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E330" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -9249,7 +9263,7 @@
         <v>345</v>
       </c>
       <c r="D331" s="31" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E331" s="40">
         <v>13</v>
@@ -9266,7 +9280,7 @@
         <v>346</v>
       </c>
       <c r="D332" s="31" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E332" s="40">
         <v>6</v>
@@ -9283,10 +9297,10 @@
         <v>347</v>
       </c>
       <c r="D333" s="31" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E333" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -9300,7 +9314,7 @@
         <v>348</v>
       </c>
       <c r="D334" s="31" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E334" s="40">
         <v>13</v>
@@ -9317,10 +9331,10 @@
         <v>349</v>
       </c>
       <c r="D335" s="31" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E335" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -9334,7 +9348,7 @@
         <v>350</v>
       </c>
       <c r="D336" s="31" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E336" s="40">
         <v>6</v>
@@ -9351,10 +9365,10 @@
         <v>351</v>
       </c>
       <c r="D337" s="31" t="s">
-        <v>872</v>
+        <v>989</v>
       </c>
       <c r="E337" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -9368,7 +9382,7 @@
         <v>352</v>
       </c>
       <c r="D338" s="31" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E338" s="40">
         <v>7</v>
@@ -9385,10 +9399,10 @@
         <v>353</v>
       </c>
       <c r="D339" s="31" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="E339" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -9402,10 +9416,10 @@
         <v>354</v>
       </c>
       <c r="D340" s="31" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="E340" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
@@ -9419,10 +9433,10 @@
         <v>355</v>
       </c>
       <c r="D341" s="31" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="E341" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
@@ -9436,7 +9450,7 @@
         <v>356</v>
       </c>
       <c r="D342" s="31" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="E342" s="40">
         <v>6</v>
@@ -9453,10 +9467,10 @@
         <v>357</v>
       </c>
       <c r="D343" s="31" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="E343" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -9470,10 +9484,10 @@
         <v>358</v>
       </c>
       <c r="D344" s="31" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="E344" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
@@ -9487,7 +9501,7 @@
         <v>359</v>
       </c>
       <c r="D345" s="31" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="E345" s="40">
         <v>7</v>
@@ -9504,10 +9518,10 @@
         <v>360</v>
       </c>
       <c r="D346" s="31" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="E346" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
@@ -9521,10 +9535,10 @@
         <v>361</v>
       </c>
       <c r="D347" s="31" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="E347" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -9538,7 +9552,7 @@
         <v>362</v>
       </c>
       <c r="D348" s="31" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="E348" s="40">
         <v>1</v>
@@ -9555,10 +9569,10 @@
         <v>363</v>
       </c>
       <c r="D349" s="31" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="E349" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -9572,7 +9586,7 @@
         <v>364</v>
       </c>
       <c r="D350" s="31" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="E350" s="40">
         <v>1</v>
@@ -9589,10 +9603,10 @@
         <v>365</v>
       </c>
       <c r="D351" s="31" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E351" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
@@ -9606,7 +9620,7 @@
         <v>366</v>
       </c>
       <c r="D352" s="31" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="E352" s="40">
         <v>6</v>
@@ -9623,7 +9637,7 @@
         <v>367</v>
       </c>
       <c r="D353" s="31" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E353" s="40">
         <v>6</v>
@@ -9640,7 +9654,7 @@
         <v>368</v>
       </c>
       <c r="D354" s="31" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="E354" s="40">
         <v>13</v>
@@ -9657,7 +9671,7 @@
         <v>369</v>
       </c>
       <c r="D355" s="31" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E355" s="40">
         <v>13</v>
@@ -9674,10 +9688,10 @@
         <v>370</v>
       </c>
       <c r="D356" s="31" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="E356" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
@@ -9691,7 +9705,7 @@
         <v>371</v>
       </c>
       <c r="D357" s="31" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E357" s="40">
         <v>13</v>
@@ -9708,7 +9722,7 @@
         <v>372</v>
       </c>
       <c r="D358" s="31" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E358" s="40">
         <v>13</v>
@@ -9725,10 +9739,10 @@
         <v>373</v>
       </c>
       <c r="D359" s="31" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E359" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
@@ -9742,10 +9756,10 @@
         <v>374</v>
       </c>
       <c r="D360" s="25" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="E360" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -9759,7 +9773,7 @@
         <v>375</v>
       </c>
       <c r="D361" s="31" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E361" s="40">
         <v>10</v>
@@ -9776,7 +9790,7 @@
         <v>376</v>
       </c>
       <c r="D362" s="31" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E362" s="40">
         <v>7</v>
@@ -9793,7 +9807,7 @@
         <v>377</v>
       </c>
       <c r="D363" s="31" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E363" s="40">
         <v>11</v>
@@ -9810,7 +9824,7 @@
         <v>378</v>
       </c>
       <c r="D364" s="31" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E364" s="40">
         <v>13</v>
@@ -9827,7 +9841,7 @@
         <v>379</v>
       </c>
       <c r="D365" s="31" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E365" s="40">
         <v>11</v>
@@ -9844,10 +9858,10 @@
         <v>380</v>
       </c>
       <c r="D366" s="31" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E366" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -9861,7 +9875,7 @@
         <v>381</v>
       </c>
       <c r="D367" s="31" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E367" s="40">
         <v>14</v>
@@ -9878,10 +9892,10 @@
         <v>382</v>
       </c>
       <c r="D368" s="31" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="E368" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -9895,10 +9909,10 @@
         <v>383</v>
       </c>
       <c r="D369" s="31" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="E369" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
@@ -9912,10 +9926,10 @@
         <v>384</v>
       </c>
       <c r="D370" s="31" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="E370" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -9929,10 +9943,10 @@
         <v>385</v>
       </c>
       <c r="D371" s="31" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="E371" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -9946,10 +9960,10 @@
         <v>386</v>
       </c>
       <c r="D372" s="31" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="E372" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
@@ -9963,7 +9977,7 @@
         <v>387</v>
       </c>
       <c r="D373" s="31" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E373" s="40">
         <v>17</v>
@@ -9980,7 +9994,7 @@
         <v>388</v>
       </c>
       <c r="D374" s="31" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="E374" s="40">
         <v>16</v>
@@ -9997,7 +10011,7 @@
         <v>389</v>
       </c>
       <c r="D375" s="31" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E375" s="40">
         <v>17</v>
@@ -10014,7 +10028,7 @@
         <v>390</v>
       </c>
       <c r="D376" s="31" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="E376" s="40">
         <v>17</v>
@@ -10031,7 +10045,7 @@
         <v>391</v>
       </c>
       <c r="D377" s="31" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="E377" s="40">
         <v>16</v>
@@ -10047,8 +10061,8 @@
       <c r="C378" s="35" t="s">
         <v>392</v>
       </c>
-      <c r="D378" s="31">
-        <v>263</v>
+      <c r="D378" s="31" t="s">
+        <v>987</v>
       </c>
       <c r="E378" s="40">
         <v>9</v>
@@ -10065,7 +10079,7 @@
         <v>393</v>
       </c>
       <c r="D379" s="31" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="E379" s="40">
         <v>9</v>
@@ -10082,7 +10096,7 @@
         <v>394</v>
       </c>
       <c r="D380" s="31" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="E380" s="40">
         <v>9</v>
@@ -10099,7 +10113,7 @@
         <v>395</v>
       </c>
       <c r="D381" s="31" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="E381" s="40">
         <v>9</v>
@@ -10116,7 +10130,7 @@
         <v>396</v>
       </c>
       <c r="D382" s="31" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="E382" s="40">
         <v>9</v>
@@ -10133,7 +10147,7 @@
         <v>397</v>
       </c>
       <c r="D383" s="31" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="E383" s="40">
         <v>17</v>
@@ -10150,7 +10164,7 @@
         <v>398</v>
       </c>
       <c r="D384" s="31" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="E384" s="40">
         <v>18</v>
@@ -10167,7 +10181,7 @@
         <v>399</v>
       </c>
       <c r="D385" s="31" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E385" s="40">
         <v>5</v>
@@ -10184,7 +10198,7 @@
         <v>400</v>
       </c>
       <c r="D386" s="31" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="E386" s="40">
         <v>1</v>
@@ -10201,10 +10215,10 @@
         <v>401</v>
       </c>
       <c r="D387" s="31" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="E387" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
@@ -10218,10 +10232,10 @@
         <v>402</v>
       </c>
       <c r="D388" s="31" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="E388" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
@@ -10235,10 +10249,10 @@
         <v>403</v>
       </c>
       <c r="D389" s="31" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E389" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
@@ -10252,7 +10266,7 @@
         <v>404</v>
       </c>
       <c r="D390" s="31" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="E390" s="40">
         <v>9</v>
@@ -10269,10 +10283,10 @@
         <v>405</v>
       </c>
       <c r="D391" s="31" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E391" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="392" spans="1:5" x14ac:dyDescent="0.25">
@@ -10286,7 +10300,7 @@
         <v>406</v>
       </c>
       <c r="D392" s="31" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="E392" s="40">
         <v>5</v>
@@ -10303,7 +10317,7 @@
         <v>407</v>
       </c>
       <c r="D393" s="31" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="E393" s="40">
         <v>14</v>
@@ -10320,7 +10334,7 @@
         <v>408</v>
       </c>
       <c r="D394" s="31" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="E394" s="40">
         <v>14</v>
@@ -10337,7 +10351,7 @@
         <v>409</v>
       </c>
       <c r="D395" s="31" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="E395" s="40">
         <v>5</v>
@@ -10354,7 +10368,7 @@
         <v>410</v>
       </c>
       <c r="D396" s="31" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="E396" s="40">
         <v>14</v>
@@ -10371,7 +10385,7 @@
         <v>411</v>
       </c>
       <c r="D397" s="31" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="E397" s="40">
         <v>14</v>
@@ -10388,10 +10402,10 @@
         <v>412</v>
       </c>
       <c r="D398" s="31" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="E398" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
@@ -10405,10 +10419,10 @@
         <v>413</v>
       </c>
       <c r="D399" s="31" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="E399" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
@@ -10422,7 +10436,7 @@
         <v>414</v>
       </c>
       <c r="D400" s="31" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="E400" s="40">
         <v>4</v>
@@ -10439,7 +10453,7 @@
         <v>415</v>
       </c>
       <c r="D401" s="31" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="E401" s="40">
         <v>4</v>
@@ -10456,7 +10470,7 @@
         <v>416</v>
       </c>
       <c r="D402" s="31" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="E402" s="40">
         <v>4</v>
@@ -10473,7 +10487,7 @@
         <v>417</v>
       </c>
       <c r="D403" s="31" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="E403" s="40">
         <v>4</v>
@@ -10490,7 +10504,7 @@
         <v>418</v>
       </c>
       <c r="D404" s="31" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="E404" s="40">
         <v>4</v>
@@ -10507,7 +10521,7 @@
         <v>419</v>
       </c>
       <c r="D405" s="31" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="E405" s="40">
         <v>16</v>
@@ -10524,7 +10538,7 @@
         <v>420</v>
       </c>
       <c r="D406" s="31" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="E406" s="40">
         <v>16</v>
@@ -10541,7 +10555,7 @@
         <v>421</v>
       </c>
       <c r="D407" s="31" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="E407" s="40">
         <v>16</v>
@@ -10558,7 +10572,7 @@
         <v>422</v>
       </c>
       <c r="D408" s="31" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="E408" s="40">
         <v>16</v>
@@ -10575,7 +10589,7 @@
         <v>423</v>
       </c>
       <c r="D409" s="31" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="E409" s="40">
         <v>16</v>
@@ -10592,7 +10606,7 @@
         <v>424</v>
       </c>
       <c r="D410" s="31" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="E410" s="40">
         <v>16</v>
@@ -10609,10 +10623,10 @@
         <v>425</v>
       </c>
       <c r="D411" s="31" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="E411" s="40" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
@@ -10626,10 +10640,10 @@
         <v>426</v>
       </c>
       <c r="D412" s="31" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="E412" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
@@ -10643,10 +10657,10 @@
         <v>427</v>
       </c>
       <c r="D413" s="31" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E413" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
@@ -10660,10 +10674,10 @@
         <v>428</v>
       </c>
       <c r="D414" s="31" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E414" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
@@ -10677,10 +10691,10 @@
         <v>429</v>
       </c>
       <c r="D415" s="31" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="E415" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
@@ -10694,10 +10708,10 @@
         <v>430</v>
       </c>
       <c r="D416" s="31" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="E416" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.25">
@@ -10711,7 +10725,7 @@
         <v>431</v>
       </c>
       <c r="D417" s="31" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="E417" s="40">
         <v>2</v>
@@ -10728,7 +10742,7 @@
         <v>432</v>
       </c>
       <c r="D418" s="31" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="E418" s="40">
         <v>2</v>
@@ -10745,7 +10759,7 @@
         <v>433</v>
       </c>
       <c r="D419" s="31" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="E419" s="40">
         <v>2</v>
@@ -10762,10 +10776,10 @@
         <v>434</v>
       </c>
       <c r="D420" s="31" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="E420" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
@@ -10779,10 +10793,10 @@
         <v>435</v>
       </c>
       <c r="D421" s="31" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="E421" s="40" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
@@ -10796,10 +10810,10 @@
         <v>436</v>
       </c>
       <c r="D422" s="31" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="E422" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
@@ -10813,7 +10827,7 @@
         <v>437</v>
       </c>
       <c r="D423" s="31" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="E423" s="40">
         <v>8</v>
@@ -10830,10 +10844,10 @@
         <v>438</v>
       </c>
       <c r="D424" s="31" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="E424" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
@@ -10847,10 +10861,10 @@
         <v>439</v>
       </c>
       <c r="D425" s="31" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="E425" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
@@ -10864,10 +10878,10 @@
         <v>440</v>
       </c>
       <c r="D426" s="31" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="E426" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
@@ -10881,10 +10895,10 @@
         <v>441</v>
       </c>
       <c r="D427" s="31" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="E427" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
@@ -10898,10 +10912,10 @@
         <v>442</v>
       </c>
       <c r="D428" s="31" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="E428" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
@@ -10915,10 +10929,10 @@
         <v>443</v>
       </c>
       <c r="D429" s="31" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="E429" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
@@ -10932,7 +10946,7 @@
         <v>444</v>
       </c>
       <c r="D430" s="31" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="E430" s="40">
         <v>8</v>
@@ -10949,10 +10963,10 @@
         <v>445</v>
       </c>
       <c r="D431" s="31" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="E431" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
@@ -10966,7 +10980,7 @@
         <v>446</v>
       </c>
       <c r="D432" s="31" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="E432" s="40">
         <v>8</v>
@@ -10983,7 +10997,7 @@
         <v>447</v>
       </c>
       <c r="D433" s="31" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="E433" s="40">
         <v>7</v>
@@ -11000,7 +11014,7 @@
         <v>448</v>
       </c>
       <c r="D434" s="31" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="E434" s="40">
         <v>7</v>
@@ -11017,7 +11031,7 @@
         <v>449</v>
       </c>
       <c r="D435" s="31" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="E435" s="40">
         <v>7</v>
@@ -11034,10 +11048,10 @@
         <v>450</v>
       </c>
       <c r="D436" s="31" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="E436" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
@@ -11051,10 +11065,10 @@
         <v>451</v>
       </c>
       <c r="D437" s="31" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="E437" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
@@ -11068,10 +11082,10 @@
         <v>452</v>
       </c>
       <c r="D438" s="31" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="E438" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
@@ -11085,7 +11099,7 @@
         <v>453</v>
       </c>
       <c r="D439" s="31" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="E439" s="40">
         <v>14</v>
@@ -11102,10 +11116,10 @@
         <v>454</v>
       </c>
       <c r="D440" s="31" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="E440" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
@@ -11119,10 +11133,10 @@
         <v>455</v>
       </c>
       <c r="D441" s="31" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="E441" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
@@ -11136,10 +11150,10 @@
         <v>456</v>
       </c>
       <c r="D442" s="31" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="E442" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
@@ -11157,7 +11171,7 @@
         <v>XL230040</v>
       </c>
       <c r="E443" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
@@ -11168,14 +11182,14 @@
         <v>10</v>
       </c>
       <c r="C444" s="38" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="D444" s="25" t="str">
         <f>VLOOKUP(C444,Sheet2!A:B,2,0)</f>
         <v>XL230041</v>
       </c>
       <c r="E444" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
@@ -11193,7 +11207,7 @@
         <v>XL230043</v>
       </c>
       <c r="E445" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
@@ -11211,7 +11225,7 @@
         <v>XL230044</v>
       </c>
       <c r="E446" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.25">
@@ -11229,7 +11243,7 @@
         <v>XL231122</v>
       </c>
       <c r="E447" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
@@ -11247,7 +11261,7 @@
         <v>XL234200</v>
       </c>
       <c r="E448" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
@@ -11265,7 +11279,7 @@
         <v>XL234430</v>
       </c>
       <c r="E449" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
@@ -11283,7 +11297,7 @@
         <v>XL235180</v>
       </c>
       <c r="E450" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
@@ -11319,7 +11333,7 @@
         <v>XL235433</v>
       </c>
       <c r="E452" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
@@ -11355,7 +11369,7 @@
         <v>XL243045</v>
       </c>
       <c r="E454" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
@@ -11369,7 +11383,7 @@
         <v>469</v>
       </c>
       <c r="D455" s="33" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="E455" s="40">
         <v>19</v>
@@ -11386,7 +11400,7 @@
         <v>470</v>
       </c>
       <c r="D456" s="33" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="E456" s="40">
         <v>19</v>
@@ -11403,7 +11417,7 @@
         <v>471</v>
       </c>
       <c r="D457" s="33" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="E457" s="40">
         <v>19</v>
@@ -11420,10 +11434,10 @@
         <v>472</v>
       </c>
       <c r="D458" s="33" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="E458" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
@@ -11437,10 +11451,10 @@
         <v>473</v>
       </c>
       <c r="D459" s="33" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="E459" s="40" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
@@ -11454,7 +11468,7 @@
         <v>474</v>
       </c>
       <c r="D460" s="33" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E460" s="40">
         <v>19</v>
@@ -11462,6 +11476,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>